<commit_message>
Added T1753 test data
</commit_message>
<xml_diff>
--- a/Test Data/T1730.xlsx
+++ b/Test Data/T1730.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1556188A-CD4C-4B0D-B118-C5537F1908E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C420CF1A-ED4B-4910-9570-47AEC4EE85AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="8" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="GalleryList" sheetId="12" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Miscellaneous" sheetId="6" r:id="rId6"/>
     <sheet name="Printers" sheetId="9" r:id="rId7"/>
     <sheet name="Accessories" sheetId="10" r:id="rId8"/>
+    <sheet name="Accessories_215 Panel" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="52">
   <si>
     <t>Wg</t>
   </si>
@@ -744,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA0CE43-C2A8-4DC2-8C6C-856D70AB4DD1}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
@@ -1437,7 +1438,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,4 +1553,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB0E2E1-6318-4988-A8FE-C1B73E6377E6}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added common test data for Belgium and Germany market
</commit_message>
<xml_diff>
--- a/Test Data/T1730.xlsx
+++ b/Test Data/T1730.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C420CF1A-ED4B-4910-9570-47AEC4EE85AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ABC28E-A2D1-4046-B481-66B1E12CFFE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="8" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="GalleryList" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="53">
   <si>
     <t>Wg</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Germany Market</t>
+  </si>
+  <si>
+    <t>FAT-S</t>
   </si>
 </sst>
 </file>
@@ -1435,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70823DFC-9F4D-48CC-8A3A-BA1CDFF79EA6}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1537,11 +1540,16 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1557,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB0E2E1-6318-4988-A8FE-C1B73E6377E6}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1644,11 +1652,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>